<commit_message>
added new strain to catalog
</commit_message>
<xml_diff>
--- a/mock catalog.xlsx
+++ b/mock catalog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>tomasensium</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>streptomyces coelicolor</t>
+  </si>
+  <si>
+    <t>tomas2</t>
   </si>
 </sst>
 </file>
@@ -348,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,6 +391,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a conflict strain
</commit_message>
<xml_diff>
--- a/mock catalog.xlsx
+++ b/mock catalog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>tomasensium</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>tomas2</t>
+  </si>
+  <si>
+    <t>tomastheBest</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +402,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>